<commit_message>
@author : kamlesh updating URL method to extract based on keyword
</commit_message>
<xml_diff>
--- a/NDC/TestSheet.xlsx
+++ b/NDC/TestSheet.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78A6B9DD-1BCC-43CF-9840-7FD41D2A7A8D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A9777D-5A9D-482B-AA63-08FE11BAA563}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="URL" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>UserName</t>
   </si>
@@ -32,6 +33,24 @@
   </si>
   <si>
     <t>kammy</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>amazon</t>
+  </si>
+  <si>
+    <t>https://amazon.co.in</t>
+  </si>
+  <si>
+    <t>google</t>
+  </si>
+  <si>
+    <t>google.co.in</t>
   </si>
 </sst>
 </file>
@@ -362,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,4 +410,50 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B629C15-A41D-44E5-8F82-F3C15D50631E}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F8C35C2B-FAFD-447C-9824-856333ADC7E5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>